<commit_message>
a lot of changes, genotypic analysis, etc.
</commit_message>
<xml_diff>
--- a/5.SH/Acer/Outputs/Multicomp_AcerSH.xlsx
+++ b/5.SH/Acer/Outputs/Multicomp_AcerSH.xlsx
@@ -205,7 +205,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -275,6 +275,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -302,7 +318,7 @@
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
+      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -594,7 +610,7 @@
       <c r="I8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="8" t="n">
+      <c r="J8" s="18" t="n">
         <f aca="false">((10^C8)-(10^C$2))/(10^C$2)</f>
         <v>-0.473663451651774</v>
       </c>
@@ -630,7 +646,7 @@
         <f aca="false">((10^C9)-(10^C$8))/(10^C$8)</f>
         <v>-0.252481881992172</v>
       </c>
-      <c r="J9" s="17" t="n">
+      <c r="J9" s="19" t="n">
         <f aca="false">((10^C9)-(10^C$3))/(10^C$3)</f>
         <v>-0.585659522447874</v>
       </c>
@@ -659,18 +675,18 @@
       <c r="G10" s="11" t="n">
         <v>-1.11230272098791</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="13" t="n">
+      <c r="I10" s="21" t="n">
         <f aca="false">((10^C10)-(10^C$8))/(10^C$8)</f>
         <v>-0.577848723435181</v>
       </c>
-      <c r="J10" s="13" t="n">
+      <c r="J10" s="21" t="n">
         <f aca="false">((10^C10)-(10^C$4))/(10^C$4)</f>
         <v>-0.722389527369984</v>
       </c>
-      <c r="K10" s="13" t="n">
+      <c r="K10" s="21" t="n">
         <f aca="false">((10^C10)-(10^C$7))/(10^C$7)</f>
         <v>-0.556722489577251</v>
       </c>
@@ -723,7 +739,7 @@
       <c r="H12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="18" t="n">
+      <c r="I12" s="22" t="n">
         <f aca="false">((10^C12)-(10^C$8))/(10^C$8)</f>
         <v>-0.774329836234245</v>
       </c>
@@ -731,7 +747,7 @@
         <f aca="false">((10^C12)-(10^C$3))/(10^C$3)</f>
         <v>-0.874913689485998</v>
       </c>
-      <c r="K12" s="9" t="n">
+      <c r="K12" s="22" t="n">
         <f aca="false">((10^C12)-(10^C$6))/(10^C$6)</f>
         <v>-0.818804354798219</v>
       </c>
@@ -759,7 +775,7 @@
       <c r="H13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="18" t="n">
+      <c r="I13" s="22" t="n">
         <f aca="false">((10^C13)-(10^C$8))/(10^C$8)</f>
         <v>-0.668219114175715</v>
       </c>
@@ -800,11 +816,11 @@
       <c r="I14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="8" t="n">
+      <c r="J14" s="18" t="n">
         <f aca="false">((10^C14)-(10^C$2))/(10^C$2)</f>
         <v>-0.803285533261645</v>
       </c>
-      <c r="K14" s="8" t="n">
+      <c r="K14" s="18" t="n">
         <f aca="false">((10^C14)-(10^C$5))/(10^C$5)</f>
         <v>-0.743215214726906</v>
       </c>
@@ -859,11 +875,11 @@
         <f aca="false">((10^C16)-(10^C$14))/(10^C$14)</f>
         <v>-0.587335530688212</v>
       </c>
-      <c r="J16" s="13" t="n">
+      <c r="J16" s="21" t="n">
         <f aca="false">((10^C16)-(10^C$4))/(10^C$4)</f>
         <v>-0.898576734841483</v>
       </c>
-      <c r="K16" s="13" t="n">
+      <c r="K16" s="21" t="n">
         <f aca="false">((10^C16)-(10^C$7))/(10^C$7)</f>
         <v>-0.838051309619245</v>
       </c>

</xml_diff>